<commit_message>
1.22 review backtrack 78,90,77,39,40,216,377
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8FB17C-49B9-E040-8D8E-55EC896BCFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5F99B-8243-AD40-9367-301776A47002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="800" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
   </bookViews>
@@ -760,12 +760,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1089,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0A4AFC-62FA-E94E-BE80-E68967C2241E}">
   <dimension ref="A1:D233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,34 +1098,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1135,10 +1134,10 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1147,10 +1146,10 @@
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1159,10 +1158,10 @@
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>387</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1171,10 +1170,10 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>383</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1183,10 +1182,10 @@
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>344</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1195,10 +1194,10 @@
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>151</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1207,10 +1206,10 @@
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1219,10 +1218,10 @@
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>345</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1231,10 +1230,10 @@
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>205</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1243,10 +1242,10 @@
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>293</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1255,10 +1254,10 @@
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>294</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1267,10 +1266,10 @@
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>290</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1279,10 +1278,10 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>242</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1291,10 +1290,10 @@
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1303,10 +1302,10 @@
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>249</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1315,10 +1314,10 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1327,10 +1326,10 @@
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>179</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1339,12 +1338,12 @@
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="8">
+      <c r="A22" s="7">
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1353,12 +1352,12 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="8">
+      <c r="A23" s="7">
         <v>161</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1367,10 +1366,10 @@
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="8">
+      <c r="A24" s="7">
         <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1379,10 +1378,10 @@
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="8">
+      <c r="A25" s="7">
         <v>358</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1391,10 +1390,10 @@
       <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
+      <c r="A26" s="7">
         <v>316</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1403,10 +1402,10 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="8">
+      <c r="A27" s="7">
         <v>271</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1415,10 +1414,10 @@
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="8">
+      <c r="A28" s="7">
         <v>168</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1427,10 +1426,10 @@
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="8">
+      <c r="A29" s="7">
         <v>171</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1439,10 +1438,10 @@
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="8">
+      <c r="A30" s="7">
         <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1451,10 +1450,10 @@
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="8">
+      <c r="A31" s="7">
         <v>12</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1463,10 +1462,10 @@
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="8">
+      <c r="A32" s="7">
         <v>273</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1475,10 +1474,10 @@
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="8">
+      <c r="A33" s="7">
         <v>246</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1487,10 +1486,10 @@
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="8"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="8">
+      <c r="A34" s="7">
         <v>247</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1499,10 +1498,10 @@
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="8"/>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="8">
+      <c r="A35" s="7">
         <v>248</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1511,20 +1510,20 @@
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="8">
+      <c r="A37" s="7">
         <v>157</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1533,10 +1532,10 @@
       <c r="C37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="8">
+      <c r="A38" s="7">
         <v>158</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1545,10 +1544,10 @@
       <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="8"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="8">
+      <c r="A39" s="7">
         <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1557,10 +1556,10 @@
       <c r="C39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="8"/>
+      <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="8">
+      <c r="A40" s="7">
         <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1569,18 +1568,18 @@
       <c r="C40" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="8"/>
+      <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="8">
+      <c r="A42" s="7">
         <v>76</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1589,12 +1588,12 @@
       <c r="C42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="8">
+      <c r="A43" s="7">
         <v>30</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1603,12 +1602,12 @@
       <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="8">
+      <c r="A44" s="7">
         <v>3</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1617,12 +1616,12 @@
       <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="8">
+      <c r="A45" s="7">
         <v>340</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1631,12 +1630,12 @@
       <c r="C45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="8">
+      <c r="A46" s="7">
         <v>395</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1645,12 +1644,12 @@
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="8">
+      <c r="A47" s="7">
         <v>159</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1659,20 +1658,20 @@
       <c r="C47" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="8">
+      <c r="A49" s="7">
         <v>125</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -1681,10 +1680,10 @@
       <c r="C49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="8"/>
+      <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="8">
+      <c r="A50" s="7">
         <v>266</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -1693,10 +1692,10 @@
       <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="8"/>
+      <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="8">
+      <c r="A51" s="7">
         <v>5</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -1705,10 +1704,10 @@
       <c r="C51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="8"/>
+      <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="8">
+      <c r="A52" s="7">
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1717,10 +1716,10 @@
       <c r="C52" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="8"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="8">
+      <c r="A53" s="7">
         <v>214</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1729,10 +1728,10 @@
       <c r="C53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="8"/>
+      <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="8">
+      <c r="A54" s="7">
         <v>336</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -1741,10 +1740,10 @@
       <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="8"/>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="8">
+      <c r="A55" s="7">
         <v>131</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -1753,10 +1752,10 @@
       <c r="C55" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="8"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="8">
+      <c r="A56" s="7">
         <v>132</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1765,10 +1764,10 @@
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="8"/>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="8">
+      <c r="A57" s="7">
         <v>267</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -1777,18 +1776,18 @@
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="8">
+      <c r="A59" s="7">
         <v>20</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -1797,10 +1796,10 @@
       <c r="C59" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="8"/>
+      <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="8">
+      <c r="A60" s="7">
         <v>22</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -1809,10 +1808,10 @@
       <c r="C60" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="8"/>
+      <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="8">
+      <c r="A61" s="7">
         <v>32</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -1821,10 +1820,10 @@
       <c r="C61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="8"/>
+      <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="8">
+      <c r="A62" s="7">
         <v>241</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -1833,10 +1832,10 @@
       <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="8"/>
+      <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="8">
+      <c r="A63" s="7">
         <v>301</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -1845,18 +1844,18 @@
       <c r="C63" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="8"/>
+      <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="8">
+      <c r="A65" s="7">
         <v>392</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -1865,10 +1864,10 @@
       <c r="C65" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="8"/>
+      <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="8">
+      <c r="A66" s="7">
         <v>115</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -1877,10 +1876,10 @@
       <c r="C66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="8"/>
+      <c r="D66" s="7"/>
     </row>
     <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="8">
+      <c r="A67" s="7">
         <v>187</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -1891,19 +1890,19 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="6" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8" t="s">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1911,7 +1910,7 @@
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -1923,7 +1922,7 @@
       <c r="A73" s="1">
         <v>94</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -1935,7 +1934,7 @@
       <c r="A74" s="1">
         <v>145</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C74" s="2" t="s">
@@ -1947,7 +1946,7 @@
       <c r="A75" s="1">
         <v>102</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
@@ -1959,7 +1958,7 @@
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="6"/>
+      <c r="B76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
@@ -1967,7 +1966,7 @@
       <c r="A77" s="1">
         <v>100</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -1979,7 +1978,7 @@
       <c r="A78" s="1">
         <v>101</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C78" s="2" t="s">
@@ -1991,7 +1990,7 @@
       <c r="A79" s="1">
         <v>226</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -2005,7 +2004,7 @@
       <c r="A80" s="1">
         <v>257</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C80" s="2" t="s">
@@ -2017,7 +2016,7 @@
       <c r="A81" s="1">
         <v>112</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C81" s="2" t="s">
@@ -2029,7 +2028,7 @@
       <c r="A82" s="1">
         <v>113</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -2041,7 +2040,7 @@
       <c r="A83" s="1">
         <v>129</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C83" s="2" t="s">
@@ -2053,7 +2052,7 @@
       <c r="A84" s="1">
         <v>298</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C84" s="2" t="s">
@@ -2065,7 +2064,7 @@
       <c r="A85" s="1">
         <v>111</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C85" s="2" t="s">
@@ -2077,7 +2076,7 @@
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="B86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
@@ -2085,7 +2084,7 @@
       <c r="A87" s="1">
         <v>104</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C87" s="2" t="s">
@@ -2097,7 +2096,7 @@
       <c r="A88" s="1">
         <v>110</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="2" t="s">
@@ -2109,7 +2108,7 @@
       <c r="A89" s="1">
         <v>124</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -2121,7 +2120,7 @@
       <c r="A90" s="1">
         <v>250</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C90" s="2" t="s">
@@ -2133,7 +2132,7 @@
       <c r="A91" s="1">
         <v>366</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -2145,7 +2144,7 @@
       <c r="A92" s="1">
         <v>337</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C92" s="2" t="s">
@@ -2159,7 +2158,7 @@
       <c r="A93" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B93" s="6"/>
+      <c r="B93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
@@ -2167,7 +2166,7 @@
       <c r="A94" s="1">
         <v>107</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
@@ -2179,7 +2178,7 @@
       <c r="A95" s="1">
         <v>103</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C95" s="2" t="s">
@@ -2191,7 +2190,7 @@
       <c r="A96" s="1">
         <v>199</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C96" s="2" t="s">
@@ -2205,7 +2204,7 @@
       <c r="A97" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B97" s="6"/>
+      <c r="B97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
@@ -2213,7 +2212,7 @@
       <c r="A98" s="1">
         <v>98</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="2" t="s">
@@ -2227,7 +2226,7 @@
       <c r="A99" s="1">
         <v>235</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C99" s="2" t="s">
@@ -2241,7 +2240,7 @@
       <c r="A100" s="1">
         <v>236</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C100" s="2" t="s">
@@ -2255,7 +2254,7 @@
       <c r="A101" s="1">
         <v>108</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C101" s="2" t="s">
@@ -2269,7 +2268,7 @@
       <c r="A102" s="1">
         <v>109</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C102" s="2" t="s">
@@ -2283,7 +2282,7 @@
       <c r="A103" s="1">
         <v>173</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C103" s="2" t="s">
@@ -2297,7 +2296,7 @@
       <c r="A104" s="1">
         <v>230</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C104" s="2" t="s">
@@ -2311,7 +2310,7 @@
       <c r="A105" s="1">
         <v>297</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C105" s="2" t="s">
@@ -2325,7 +2324,7 @@
       <c r="A106" s="1">
         <v>285</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C106" s="2" t="s">
@@ -2339,7 +2338,7 @@
       <c r="A107" s="1">
         <v>270</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C107" s="2" t="s">
@@ -2353,7 +2352,7 @@
       <c r="A108" s="1">
         <v>272</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C108" s="2" t="s">
@@ -2367,7 +2366,7 @@
       <c r="A109" s="1">
         <v>99</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C109" s="2" t="s">
@@ -2381,7 +2380,7 @@
       <c r="A110" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B110" s="4"/>
+      <c r="B110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
@@ -2389,7 +2388,7 @@
       <c r="A111" s="1">
         <v>116</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -2403,7 +2402,7 @@
       <c r="A112" s="1">
         <v>117</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -2417,7 +2416,7 @@
       <c r="A113" s="1">
         <v>314</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C113" s="2" t="s">
@@ -2431,7 +2430,7 @@
       <c r="A114" s="1">
         <v>96</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C114" s="2" t="s">
@@ -2442,34 +2441,34 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B115" s="10"/>
+      <c r="B115" s="9"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B116" s="10"/>
+      <c r="B116" s="9"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B117" s="10"/>
+      <c r="B117" s="9"/>
     </row>
     <row r="118" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B118" s="10"/>
+      <c r="B118" s="9"/>
     </row>
     <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B119" s="9"/>
-      <c r="C119" s="8" t="s">
+      <c r="B119" s="8"/>
+      <c r="C119" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D119" s="8" t="s">
+      <c r="D119" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="8">
+      <c r="A120" s="7">
         <v>78</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -2478,10 +2477,10 @@
       <c r="C120" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D120" s="8"/>
+      <c r="D120" s="7"/>
     </row>
     <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="8">
+      <c r="A121" s="7">
         <v>90</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -2490,10 +2489,10 @@
       <c r="C121" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D121" s="8"/>
+      <c r="D121" s="7"/>
     </row>
     <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="8">
+      <c r="A122" s="7">
         <v>77</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -2502,10 +2501,10 @@
       <c r="C122" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D122" s="8"/>
+      <c r="D122" s="7"/>
     </row>
     <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="8">
+      <c r="A123" s="7">
         <v>39</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -2514,10 +2513,10 @@
       <c r="C123" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D123" s="8"/>
+      <c r="D123" s="7"/>
     </row>
     <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="8">
+      <c r="A124" s="7">
         <v>40</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -2526,10 +2525,10 @@
       <c r="C124" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D124" s="8"/>
+      <c r="D124" s="7"/>
     </row>
     <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="8">
+      <c r="A125" s="7">
         <v>216</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -2538,10 +2537,10 @@
       <c r="C125" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D125" s="8"/>
+      <c r="D125" s="7"/>
     </row>
     <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="8">
+      <c r="A126" s="7">
         <v>377</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -2550,12 +2549,12 @@
       <c r="C126" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D126" s="8" t="s">
+      <c r="D126" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="8">
+      <c r="A127" s="7">
         <v>254</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -2564,10 +2563,10 @@
       <c r="C127" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D127" s="8"/>
+      <c r="D127" s="7"/>
     </row>
     <row r="128" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="8">
+      <c r="A128" s="7">
         <v>46</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -2576,749 +2575,749 @@
       <c r="C128" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D128" s="8"/>
+      <c r="D128" s="7"/>
     </row>
     <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="8">
+      <c r="A129" s="7">
         <v>47</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="B129" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D129" s="8"/>
+      <c r="D129" s="7"/>
     </row>
     <row r="130" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="8">
+      <c r="A130" s="7">
         <v>31</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D130" s="8" t="s">
+      <c r="D130" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="8">
+      <c r="A131" s="7">
         <v>60</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D131" s="8" t="s">
+      <c r="D131" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="8">
+      <c r="A132" s="7">
         <v>291</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D132" s="8"/>
+      <c r="D132" s="7"/>
     </row>
     <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="8">
+      <c r="A133" s="7">
         <v>17</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D133" s="8"/>
+      <c r="D133" s="7"/>
     </row>
     <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A134" s="8">
+      <c r="A134" s="7">
         <v>320</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="B134" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D134" s="8"/>
+      <c r="D134" s="7"/>
     </row>
     <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="8">
+      <c r="A135" s="7">
         <v>282</v>
       </c>
-      <c r="B135" s="5" t="s">
+      <c r="B135" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D135" s="8"/>
+      <c r="D135" s="7"/>
     </row>
     <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" s="8">
+      <c r="A136" s="7">
         <v>140</v>
       </c>
-      <c r="B136" s="5" t="s">
+      <c r="B136" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D136" s="8"/>
+      <c r="D136" s="7"/>
     </row>
     <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="8">
+      <c r="A137" s="7">
         <v>351</v>
       </c>
-      <c r="B137" s="5" t="s">
+      <c r="B137" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A140" s="7" t="s">
+      <c r="A140" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="8" t="s">
+      <c r="A141" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B141" s="8"/>
-      <c r="C141" s="8" t="s">
+      <c r="B141" s="7"/>
+      <c r="C141" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D141" s="8" t="s">
+      <c r="D141" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="8" t="s">
+      <c r="A142" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B142" s="8"/>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="7"/>
+      <c r="D142" s="7"/>
     </row>
     <row r="143" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="8">
+      <c r="A143" s="7">
         <v>70</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="B143" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D143" s="8"/>
+      <c r="D143" s="7"/>
     </row>
     <row r="144" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A144" s="8">
+      <c r="A144" s="7">
         <v>62</v>
       </c>
-      <c r="B144" s="5" t="s">
+      <c r="B144" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D144" s="8"/>
+      <c r="D144" s="7"/>
     </row>
     <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A145" s="8">
+      <c r="A145" s="7">
         <v>63</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B145" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D145" s="8"/>
+      <c r="D145" s="7"/>
     </row>
     <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A146" s="8">
+      <c r="A146" s="7">
         <v>279</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D146" s="8"/>
+      <c r="D146" s="7"/>
     </row>
     <row r="147" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" s="8">
+      <c r="A147" s="7">
         <v>139</v>
       </c>
-      <c r="B147" s="5" t="s">
+      <c r="B147" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D147" s="8"/>
+      <c r="D147" s="7"/>
     </row>
     <row r="148" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A148" s="8">
+      <c r="A148" s="7">
         <v>375</v>
       </c>
-      <c r="B148" s="5" t="s">
+      <c r="B148" s="4" t="s">
         <v>82</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D148" s="8"/>
+      <c r="D148" s="7"/>
     </row>
     <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" s="8">
+      <c r="A149" s="7">
         <v>312</v>
       </c>
-      <c r="B149" s="5" t="s">
+      <c r="B149" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D149" s="8"/>
+      <c r="D149" s="7"/>
     </row>
     <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" s="8">
+      <c r="A150" s="7">
         <v>322</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B150" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D150" s="8"/>
+      <c r="D150" s="7"/>
     </row>
     <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" s="8" t="s">
+      <c r="A151" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B151" s="9"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="7"/>
+      <c r="D151" s="7"/>
     </row>
     <row r="152" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="8">
+      <c r="A152" s="7">
         <v>256</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D152" s="8"/>
+      <c r="D152" s="7"/>
     </row>
     <row r="153" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="8">
+      <c r="A153" s="7">
         <v>265</v>
       </c>
-      <c r="B153" s="5" t="s">
+      <c r="B153" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D153" s="8"/>
+      <c r="D153" s="7"/>
     </row>
     <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" s="8">
+      <c r="A154" s="7">
         <v>64</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D154" s="8"/>
+      <c r="D154" s="7"/>
     </row>
     <row r="155" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" s="8">
+      <c r="A155" s="7">
         <v>72</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B155" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D155" s="8"/>
+      <c r="D155" s="7"/>
     </row>
     <row r="156" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="8">
+      <c r="A156" s="7">
         <v>97</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="4" t="s">
         <v>90</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D156" s="8"/>
+      <c r="D156" s="7"/>
     </row>
     <row r="157" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="8">
+      <c r="A157" s="7">
         <v>174</v>
       </c>
-      <c r="B157" s="5" t="s">
+      <c r="B157" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D157" s="8"/>
+      <c r="D157" s="7"/>
     </row>
     <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="8">
+      <c r="A158" s="7">
         <v>221</v>
       </c>
-      <c r="B158" s="5" t="s">
+      <c r="B158" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D158" s="8"/>
+      <c r="D158" s="7"/>
     </row>
     <row r="159" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="8">
+      <c r="A159" s="7">
         <v>85</v>
       </c>
-      <c r="B159" s="5" t="s">
+      <c r="B159" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D159" s="8"/>
+      <c r="D159" s="7"/>
     </row>
     <row r="160" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="8">
+      <c r="A160" s="7">
         <v>363</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="4" t="s">
         <v>94</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D160" s="8" t="s">
+      <c r="D160" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="8" t="s">
+      <c r="A161" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B161" s="9"/>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
+      <c r="B161" s="8"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
     </row>
     <row r="162" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="8">
+      <c r="A162" s="7">
         <v>198</v>
       </c>
-      <c r="B162" s="5" t="s">
+      <c r="B162" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D162" s="8"/>
+      <c r="D162" s="7"/>
     </row>
     <row r="163" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="8">
+      <c r="A163" s="7">
         <v>213</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B163" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D163" s="8"/>
+      <c r="D163" s="7"/>
     </row>
     <row r="164" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A164" s="8">
+      <c r="A164" s="7">
         <v>276</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B164" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D164" s="8"/>
+      <c r="D164" s="7"/>
     </row>
     <row r="165" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="8">
+      <c r="A165" s="7">
         <v>91</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B165" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D165" s="8"/>
+      <c r="D165" s="7"/>
     </row>
     <row r="166" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" s="8">
+      <c r="A166" s="7">
         <v>10</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B166" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D166" s="8"/>
+      <c r="D166" s="7"/>
     </row>
     <row r="167" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="8">
+      <c r="A167" s="7">
         <v>44</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B167" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A170" s="7" t="s">
+      <c r="A170" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A171" s="8" t="s">
+      <c r="A171" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B171" s="8"/>
-      <c r="C171" s="8" t="s">
+      <c r="B171" s="7"/>
+      <c r="C171" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A172" s="8" t="s">
+      <c r="A172" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B172" s="8"/>
-      <c r="C172" s="8"/>
-      <c r="D172" s="8"/>
+      <c r="B172" s="7"/>
+      <c r="C172" s="7"/>
+      <c r="D172" s="7"/>
     </row>
     <row r="173" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="8">
+      <c r="A173" s="7">
         <v>206</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="B173" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D173" s="8"/>
+      <c r="D173" s="7"/>
     </row>
     <row r="174" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A174" s="8">
+      <c r="A174" s="7">
         <v>141</v>
       </c>
-      <c r="B174" s="5" t="s">
+      <c r="B174" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D174" s="8"/>
+      <c r="D174" s="7"/>
     </row>
     <row r="175" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="8">
+      <c r="A175" s="7">
         <v>24</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="B175" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D175" s="8"/>
+      <c r="D175" s="7"/>
     </row>
     <row r="176" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A176" s="8">
+      <c r="A176" s="7">
         <v>328</v>
       </c>
-      <c r="B176" s="5" t="s">
+      <c r="B176" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D176" s="8"/>
+      <c r="D176" s="7"/>
     </row>
     <row r="177" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A177" s="8">
+      <c r="A177" s="7">
         <v>92</v>
       </c>
-      <c r="B177" s="5" t="s">
+      <c r="B177" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D177" s="8"/>
+      <c r="D177" s="7"/>
     </row>
     <row r="178" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" s="8">
+      <c r="A178" s="7">
         <v>237</v>
       </c>
-      <c r="B178" s="5" t="s">
+      <c r="B178" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D178" s="8"/>
+      <c r="D178" s="7"/>
     </row>
     <row r="179" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A179" s="8">
+      <c r="A179" s="7">
         <v>19</v>
       </c>
-      <c r="B179" s="5" t="s">
+      <c r="B179" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D179" s="8"/>
+      <c r="D179" s="7"/>
     </row>
     <row r="180" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" s="8">
+      <c r="A180" s="7">
         <v>83</v>
       </c>
-      <c r="B180" s="5" t="s">
+      <c r="B180" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D180" s="8"/>
+      <c r="D180" s="7"/>
     </row>
     <row r="181" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A181" s="8">
+      <c r="A181" s="7">
         <v>203</v>
       </c>
-      <c r="B181" s="5" t="s">
+      <c r="B181" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D181" s="8"/>
+      <c r="D181" s="7"/>
     </row>
     <row r="182" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="8">
+      <c r="A182" s="7">
         <v>82</v>
       </c>
-      <c r="B182" s="5" t="s">
+      <c r="B182" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="8"/>
+      <c r="D182" s="7"/>
     </row>
     <row r="183" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="8">
+      <c r="A183" s="7">
         <v>369</v>
       </c>
-      <c r="B183" s="5" t="s">
+      <c r="B183" s="4" t="s">
         <v>115</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D183" s="8"/>
+      <c r="D183" s="7"/>
     </row>
     <row r="184" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A184" s="8">
-        <v>2</v>
-      </c>
-      <c r="B184" s="5" t="s">
+      <c r="A184" s="7">
+        <v>2</v>
+      </c>
+      <c r="B184" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D184" s="8"/>
+      <c r="D184" s="7"/>
     </row>
     <row r="185" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="8">
+      <c r="A185" s="7">
         <v>160</v>
       </c>
-      <c r="B185" s="5" t="s">
+      <c r="B185" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D185" s="8"/>
+      <c r="D185" s="7"/>
     </row>
     <row r="186" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" s="8">
+      <c r="A186" s="7">
         <v>21</v>
       </c>
-      <c r="B186" s="5" t="s">
+      <c r="B186" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D186" s="8"/>
+      <c r="D186" s="7"/>
     </row>
     <row r="187" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A187" s="8" t="s">
+      <c r="A187" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B187" s="9"/>
-      <c r="C187" s="8"/>
-      <c r="D187" s="8"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
     </row>
     <row r="188" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A188" s="8">
+      <c r="A188" s="7">
         <v>234</v>
       </c>
-      <c r="B188" s="5" t="s">
+      <c r="B188" s="4" t="s">
         <v>120</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D188" s="8"/>
+      <c r="D188" s="7"/>
     </row>
     <row r="189" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A189" s="8">
+      <c r="A189" s="7">
         <v>143</v>
       </c>
-      <c r="B189" s="5" t="s">
+      <c r="B189" s="4" t="s">
         <v>121</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D189" s="8"/>
+      <c r="D189" s="7"/>
     </row>
     <row r="190" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A190" s="8">
+      <c r="A190" s="7">
         <v>142</v>
       </c>
-      <c r="B190" s="5" t="s">
+      <c r="B190" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D190" s="8"/>
+      <c r="D190" s="7"/>
     </row>
     <row r="191" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A191" s="8">
+      <c r="A191" s="7">
         <v>148</v>
       </c>
-      <c r="B191" s="5" t="s">
+      <c r="B191" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D191" s="8"/>
+      <c r="D191" s="7"/>
     </row>
     <row r="192" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A192" s="8">
+      <c r="A192" s="7">
         <v>25</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="B192" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D192" s="8"/>
+      <c r="D192" s="7"/>
     </row>
     <row r="193" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A193" s="8">
+      <c r="A193" s="7">
         <v>61</v>
       </c>
-      <c r="B193" s="5" t="s">
+      <c r="B193" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D193" s="8"/>
+      <c r="D193" s="7"/>
     </row>
     <row r="194" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A194" s="8">
+      <c r="A194" s="7">
         <v>86</v>
       </c>
-      <c r="B194" s="5" t="s">
+      <c r="B194" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D194" s="8"/>
+      <c r="D194" s="7"/>
     </row>
     <row r="195" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" s="8">
+      <c r="A195" s="7">
         <v>23</v>
       </c>
-      <c r="B195" s="5" t="s">
+      <c r="B195" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D195" s="8"/>
+      <c r="D195" s="7"/>
     </row>
     <row r="196" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="8">
+      <c r="A196" s="7">
         <v>147</v>
       </c>
-      <c r="B196" s="5" t="s">
+      <c r="B196" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A199" s="7" t="s">
+      <c r="A199" s="6" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A200" s="8" t="s">
+      <c r="A200" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B200" s="8"/>
-      <c r="C200" s="8" t="s">
+      <c r="B200" s="7"/>
+      <c r="C200" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A201" s="8">
+      <c r="A201" s="7">
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
@@ -3327,10 +3326,10 @@
       <c r="C201" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D201" s="8"/>
+      <c r="D201" s="7"/>
     </row>
     <row r="202" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A202" s="8">
+      <c r="A202" s="7">
         <v>286</v>
       </c>
       <c r="B202" s="2" t="s">
@@ -3339,245 +3338,245 @@
       <c r="C202" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D202" s="8"/>
+      <c r="D202" s="7"/>
     </row>
     <row r="203" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A203" s="8">
+      <c r="A203" s="7">
         <v>130</v>
       </c>
-      <c r="B203" s="5" t="s">
+      <c r="B203" s="4" t="s">
         <v>132</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D203" s="8"/>
+      <c r="D203" s="7"/>
     </row>
     <row r="204" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A204" s="8">
+      <c r="A204" s="7">
         <v>339</v>
       </c>
-      <c r="B204" s="5" t="s">
+      <c r="B204" s="4" t="s">
         <v>133</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D204" s="8"/>
+      <c r="D204" s="7"/>
     </row>
     <row r="205" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A205" s="8">
+      <c r="A205" s="7">
         <v>364</v>
       </c>
-      <c r="B205" s="5" t="s">
+      <c r="B205" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D205" s="8"/>
+      <c r="D205" s="7"/>
     </row>
     <row r="206" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A206" s="8">
+      <c r="A206" s="7">
         <v>127</v>
       </c>
-      <c r="B206" s="5" t="s">
+      <c r="B206" s="4" t="s">
         <v>135</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D206" s="8"/>
+      <c r="D206" s="7"/>
     </row>
     <row r="207" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A207" s="8">
+      <c r="A207" s="7">
         <v>51</v>
       </c>
-      <c r="B207" s="5" t="s">
+      <c r="B207" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D207" s="8"/>
+      <c r="D207" s="7"/>
     </row>
     <row r="208" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A208" s="8">
+      <c r="A208" s="7">
         <v>52</v>
       </c>
-      <c r="B208" s="5" t="s">
+      <c r="B208" s="4" t="s">
         <v>137</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D208" s="8"/>
+      <c r="D208" s="7"/>
     </row>
     <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A209" s="8">
+      <c r="A209" s="7">
         <v>126</v>
       </c>
-      <c r="B209" s="5" t="s">
+      <c r="B209" s="4" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B210" s="10"/>
+      <c r="B210" s="9"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B211" s="10"/>
+      <c r="B211" s="9"/>
     </row>
     <row r="212" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A212" s="7" t="s">
+      <c r="A212" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B212" s="10"/>
+      <c r="B212" s="9"/>
     </row>
     <row r="213" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A213" s="8" t="s">
+      <c r="A213" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B213" s="9"/>
-      <c r="C213" s="8" t="s">
+      <c r="B213" s="8"/>
+      <c r="C213" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A214" s="8">
+      <c r="A214" s="7">
         <v>261</v>
       </c>
-      <c r="B214" s="5" t="s">
+      <c r="B214" s="4" t="s">
         <v>140</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D214" s="8"/>
+      <c r="D214" s="7"/>
     </row>
     <row r="215" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A215" s="8">
+      <c r="A215" s="7">
         <v>323</v>
       </c>
-      <c r="B215" s="5" t="s">
+      <c r="B215" s="4" t="s">
         <v>141</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D215" s="8"/>
+      <c r="D215" s="7"/>
     </row>
     <row r="216" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A216" s="8">
+      <c r="A216" s="7">
         <v>305</v>
       </c>
-      <c r="B216" s="5" t="s">
+      <c r="B216" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B217" s="10"/>
+      <c r="B217" s="9"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B218" s="10"/>
+      <c r="B218" s="9"/>
     </row>
     <row r="219" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A219" s="7" t="s">
+      <c r="A219" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B219" s="10"/>
+      <c r="B219" s="9"/>
     </row>
     <row r="220" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A220" s="8" t="s">
+      <c r="A220" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B220" s="9"/>
-      <c r="C220" s="8" t="s">
+      <c r="B220" s="8"/>
+      <c r="C220" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D220" s="8" t="s">
+      <c r="D220" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A221" s="8" t="s">
+      <c r="A221" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B221" s="9"/>
-      <c r="C221" s="8"/>
-      <c r="D221" s="8"/>
+      <c r="B221" s="8"/>
+      <c r="C221" s="7"/>
+      <c r="D221" s="7"/>
     </row>
     <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A222" s="8">
+      <c r="A222" s="7">
         <v>133</v>
       </c>
-      <c r="B222" s="5" t="s">
+      <c r="B222" s="4" t="s">
         <v>211</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D222" s="8"/>
+      <c r="D222" s="7"/>
     </row>
     <row r="223" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A223" s="8">
+      <c r="A223" s="7">
         <v>399</v>
       </c>
-      <c r="B223" s="5" t="s">
+      <c r="B223" s="4" t="s">
         <v>212</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D223" s="8"/>
+      <c r="D223" s="7"/>
     </row>
     <row r="224" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A224" s="8">
+      <c r="A224" s="7">
         <v>310</v>
       </c>
-      <c r="B224" s="5" t="s">
+      <c r="B224" s="4" t="s">
         <v>213</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D224" s="8"/>
+      <c r="D224" s="7"/>
     </row>
     <row r="225" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A225" s="8" t="s">
+      <c r="A225" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B225" s="9"/>
-      <c r="C225" s="8"/>
-      <c r="D225" s="8"/>
+      <c r="B225" s="8"/>
+      <c r="C225" s="7"/>
+      <c r="D225" s="7"/>
     </row>
     <row r="226" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A226" s="8">
+      <c r="A226" s="7">
         <v>149</v>
       </c>
-      <c r="B226" s="5" t="s">
+      <c r="B226" s="4" t="s">
         <v>215</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D226" s="8"/>
+      <c r="D226" s="7"/>
     </row>
     <row r="229" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A229" s="7" t="s">
+      <c r="A229" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A230" s="8" t="s">
+      <c r="A230" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B230" s="8"/>
-      <c r="C230" s="8" t="s">
+      <c r="B230" s="7"/>
+      <c r="C230" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A231" s="8">
+      <c r="A231" s="7">
         <v>211</v>
       </c>
       <c r="B231" s="2" t="s">
@@ -3586,10 +3585,10 @@
       <c r="C231" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D231" s="8"/>
+      <c r="D231" s="7"/>
     </row>
     <row r="232" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A232" s="8">
+      <c r="A232" s="7">
         <v>208</v>
       </c>
       <c r="B232" s="2" t="s">
@@ -3598,10 +3597,10 @@
       <c r="C232" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D232" s="8"/>
+      <c r="D232" s="7"/>
     </row>
     <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A233" s="8">
+      <c r="A233" s="7">
         <v>212</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -3610,7 +3609,7 @@
       <c r="C233" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D233" s="8"/>
+      <c r="D233" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>